<commit_message>
Updates from Sadia- 10th April
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prith\IdeaProjects\AutomationFW3\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MISS. SADIA NASIM\IdeaProjects\AutomationFW3\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6C7155-2839-4482-B26C-C0170DCFCB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{4573A118-7407-48E8-A8DF-2895DBFDB4EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="24888" windowHeight="14916"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -110,12 +109,39 @@
   </si>
   <si>
     <t>Products</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>ExpectedCount</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>PriceTag</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>SortValue</t>
+  </si>
+  <si>
+    <t>az</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -466,20 +492,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C632C3F5-C571-48A2-9929-A703EEF96349}">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -504,8 +530,17 @@
       <c r="H1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -519,7 +554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -536,7 +571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -550,7 +585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -570,7 +605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -587,7 +622,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -604,7 +639,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -619,6 +654,71 @@
       </c>
       <c r="H8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates from Sadia- 21st April
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>az</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>za</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,6 +727,23 @@
         <v>33</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates from Sadia- 27thApril
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -142,6 +142,21 @@
   </si>
   <si>
     <t>za</t>
+  </si>
+  <si>
+    <t>TC_011</t>
+  </si>
+  <si>
+    <t>lohi</t>
+  </si>
+  <si>
+    <t>TC_012</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bike Light</t>
   </si>
 </sst>
 </file>
@@ -499,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +526,7 @@
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -545,8 +560,11 @@
       <c r="K1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -560,7 +578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -577,7 +595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -591,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -611,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -628,7 +646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -645,7 +663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -662,7 +680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -676,7 +694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -693,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -710,7 +728,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -727,7 +745,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -742,6 +760,40 @@
       </c>
       <c r="K13" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates from Sadia- 17thMay
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -156,7 +156,40 @@
     <t>ItemName</t>
   </si>
   <si>
+    <t>hilo</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
     <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>Sadia</t>
+  </si>
+  <si>
+    <t>Nasim</t>
   </si>
 </sst>
 </file>
@@ -514,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,7 +559,7 @@
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -563,8 +596,17 @@
       <c r="L1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -578,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -595,7 +637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -609,7 +651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -629,7 +671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -646,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -663,7 +705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -680,7 +722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -694,7 +736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -711,7 +753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -728,7 +770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -745,7 +787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -762,7 +804,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -779,7 +821,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -792,12 +834,73 @@
       <c r="D15" t="s">
         <v>17</v>
       </c>
-      <c r="L15" t="s">
+      <c r="K15" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18">
+        <v>711101</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>